<commit_message>
update lactic acid biorefinery
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/lactic/results/0_baseline.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/lactic/results/0_baseline.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yalinli_cabbi/Library/CloudStorage/OneDrive-Personal/Coding/bp/BioSTEAM 2.x.x/biorefineries/lactic/results/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17A33F8-5420-5742-A285-B86102F71313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="11040" yWindow="3980" windowWidth="28420" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -328,24 +334,6 @@
     <t>Check [10^6 kJ/hr]</t>
   </si>
   <si>
-    <t>pretreatment_group [10^9 kJ/yr]</t>
-  </si>
-  <si>
-    <t>conversion_group [10^9 kJ/yr]</t>
-  </si>
-  <si>
-    <t>separation_group [10^9 kJ/yr]</t>
-  </si>
-  <si>
-    <t>wastewater_group [10^9 kJ/yr]</t>
-  </si>
-  <si>
-    <t>CHP_group [10^9 kJ/yr]</t>
-  </si>
-  <si>
-    <t>facilities_no_hu_group [10^9 kJ/yr]</t>
-  </si>
-  <si>
     <t>CT [10^6 kJ/hr]</t>
   </si>
   <si>
@@ -452,13 +440,31 @@
   </si>
   <si>
     <t>end</t>
+  </si>
+  <si>
+    <t>pretreatment_group [10^6 kJ/yr]</t>
+  </si>
+  <si>
+    <t>conversion_group [10^6 kJ/yr]</t>
+  </si>
+  <si>
+    <t>separation_group [10^6 kJ/yr]</t>
+  </si>
+  <si>
+    <t>wastewater_group [10^6 kJ/yr]</t>
+  </si>
+  <si>
+    <t>CHP_group [10^6 kJ/yr]</t>
+  </si>
+  <si>
+    <t>facilities_no_hu_group [10^6 kJ/yr]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -510,8 +516,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -521,6 +530,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -567,7 +584,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -599,9 +616,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -633,6 +668,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -808,301 +861,303 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:FW5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="AX14" sqref="AX14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:179">
+    <row r="1" spans="1:179" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1" t="s">
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
-      <c r="AC1" s="1"/>
-      <c r="AD1" s="1"/>
-      <c r="AE1" s="1"/>
-      <c r="AF1" s="1"/>
-      <c r="AG1" s="1"/>
-      <c r="AH1" s="1"/>
-      <c r="AI1" s="1"/>
-      <c r="AJ1" s="1"/>
-      <c r="AK1" s="1"/>
-      <c r="AL1" s="1"/>
-      <c r="AM1" s="1"/>
-      <c r="AN1" s="1" t="s">
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="2"/>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="2"/>
+      <c r="AI1" s="2"/>
+      <c r="AJ1" s="2"/>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="2"/>
+      <c r="AM1" s="2"/>
+      <c r="AN1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AO1" s="1"/>
-      <c r="AP1" s="1"/>
-      <c r="AQ1" s="1"/>
-      <c r="AR1" s="1" t="s">
+      <c r="AO1" s="2"/>
+      <c r="AP1" s="2"/>
+      <c r="AQ1" s="2"/>
+      <c r="AR1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="AS1" s="1"/>
-      <c r="AT1" s="1"/>
-      <c r="AU1" s="1"/>
-      <c r="AV1" s="1"/>
-      <c r="AW1" s="1"/>
-      <c r="AX1" s="1"/>
-      <c r="AY1" s="1"/>
-      <c r="AZ1" s="1"/>
-      <c r="BA1" s="1"/>
-      <c r="BB1" s="1" t="s">
+      <c r="AS1" s="2"/>
+      <c r="AT1" s="2"/>
+      <c r="AU1" s="2"/>
+      <c r="AV1" s="2"/>
+      <c r="AW1" s="2"/>
+      <c r="AX1" s="2"/>
+      <c r="AY1" s="2"/>
+      <c r="AZ1" s="2"/>
+      <c r="BA1" s="2"/>
+      <c r="BB1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="BC1" s="1"/>
-      <c r="BD1" s="1"/>
-      <c r="BE1" s="1"/>
-      <c r="BF1" s="1"/>
-      <c r="BG1" s="1"/>
-      <c r="BH1" s="1"/>
-      <c r="BI1" s="1"/>
-      <c r="BJ1" s="1"/>
-      <c r="BK1" s="1"/>
-      <c r="BL1" s="1" t="s">
+      <c r="BC1" s="2"/>
+      <c r="BD1" s="2"/>
+      <c r="BE1" s="2"/>
+      <c r="BF1" s="2"/>
+      <c r="BG1" s="2"/>
+      <c r="BH1" s="2"/>
+      <c r="BI1" s="2"/>
+      <c r="BJ1" s="2"/>
+      <c r="BK1" s="2"/>
+      <c r="BL1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="BM1" s="1"/>
-      <c r="BN1" s="1"/>
-      <c r="BO1" s="1"/>
-      <c r="BP1" s="1"/>
-      <c r="BQ1" s="1"/>
-      <c r="BR1" s="1"/>
-      <c r="BS1" s="1"/>
-      <c r="BT1" s="1"/>
-      <c r="BU1" s="1"/>
-      <c r="BV1" s="1" t="s">
+      <c r="BM1" s="2"/>
+      <c r="BN1" s="2"/>
+      <c r="BO1" s="2"/>
+      <c r="BP1" s="2"/>
+      <c r="BQ1" s="2"/>
+      <c r="BR1" s="2"/>
+      <c r="BS1" s="2"/>
+      <c r="BT1" s="2"/>
+      <c r="BU1" s="2"/>
+      <c r="BV1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="BW1" s="1"/>
-      <c r="BX1" s="1"/>
-      <c r="BY1" s="1"/>
-      <c r="BZ1" s="1"/>
-      <c r="CA1" s="1"/>
-      <c r="CB1" s="1"/>
-      <c r="CC1" s="1"/>
-      <c r="CD1" s="1"/>
-      <c r="CE1" s="1"/>
+      <c r="BW1" s="2"/>
+      <c r="BX1" s="2"/>
+      <c r="BY1" s="2"/>
+      <c r="BZ1" s="2"/>
+      <c r="CA1" s="2"/>
+      <c r="CB1" s="2"/>
+      <c r="CC1" s="2"/>
+      <c r="CD1" s="2"/>
+      <c r="CE1" s="2"/>
       <c r="CF1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="CG1" s="1" t="s">
+      <c r="CG1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="CH1" s="1"/>
-      <c r="CI1" s="1" t="s">
+      <c r="CH1" s="2"/>
+      <c r="CI1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="CJ1" s="1"/>
-      <c r="CK1" s="1" t="s">
+      <c r="CJ1" s="2"/>
+      <c r="CK1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="CL1" s="1"/>
-      <c r="CM1" s="1" t="s">
+      <c r="CL1" s="2"/>
+      <c r="CM1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="CN1" s="1"/>
-      <c r="CO1" s="1" t="s">
+      <c r="CN1" s="2"/>
+      <c r="CO1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="CP1" s="1"/>
-      <c r="CQ1" s="1" t="s">
+      <c r="CP1" s="2"/>
+      <c r="CQ1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="CR1" s="1"/>
-      <c r="CS1" s="1" t="s">
+      <c r="CR1" s="2"/>
+      <c r="CS1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="CT1" s="1"/>
-      <c r="CU1" s="1" t="s">
+      <c r="CT1" s="2"/>
+      <c r="CU1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="CV1" s="1"/>
-      <c r="CW1" s="1" t="s">
+      <c r="CV1" s="2"/>
+      <c r="CW1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="CX1" s="1"/>
-      <c r="CY1" s="1" t="s">
+      <c r="CX1" s="2"/>
+      <c r="CY1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="CZ1" s="1"/>
-      <c r="DA1" s="1" t="s">
+      <c r="CZ1" s="2"/>
+      <c r="DA1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="DB1" s="1"/>
-      <c r="DC1" s="1" t="s">
+      <c r="DB1" s="2"/>
+      <c r="DC1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="DD1" s="1"/>
-      <c r="DE1" s="1" t="s">
+      <c r="DD1" s="2"/>
+      <c r="DE1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="DF1" s="1"/>
-      <c r="DG1" s="1" t="s">
+      <c r="DF1" s="2"/>
+      <c r="DG1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="DH1" s="1"/>
-      <c r="DI1" s="1" t="s">
+      <c r="DH1" s="2"/>
+      <c r="DI1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="DJ1" s="1"/>
-      <c r="DK1" s="1" t="s">
+      <c r="DJ1" s="2"/>
+      <c r="DK1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="DL1" s="1"/>
-      <c r="DM1" s="1" t="s">
+      <c r="DL1" s="2"/>
+      <c r="DM1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="DN1" s="1"/>
-      <c r="DO1" s="1" t="s">
+      <c r="DN1" s="2"/>
+      <c r="DO1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="DP1" s="1"/>
-      <c r="DQ1" s="1" t="s">
+      <c r="DP1" s="2"/>
+      <c r="DQ1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="DR1" s="1"/>
-      <c r="DS1" s="1" t="s">
+      <c r="DR1" s="2"/>
+      <c r="DS1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="DT1" s="1"/>
-      <c r="DU1" s="1" t="s">
+      <c r="DT1" s="2"/>
+      <c r="DU1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="DV1" s="1"/>
-      <c r="DW1" s="1" t="s">
+      <c r="DV1" s="2"/>
+      <c r="DW1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="DX1" s="1"/>
-      <c r="DY1" s="1" t="s">
+      <c r="DX1" s="2"/>
+      <c r="DY1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="DZ1" s="1"/>
-      <c r="EA1" s="1" t="s">
+      <c r="DZ1" s="2"/>
+      <c r="EA1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="EB1" s="1"/>
-      <c r="EC1" s="1" t="s">
+      <c r="EB1" s="2"/>
+      <c r="EC1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="ED1" s="1"/>
-      <c r="EE1" s="1" t="s">
+      <c r="ED1" s="2"/>
+      <c r="EE1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="EF1" s="1"/>
-      <c r="EG1" s="1" t="s">
+      <c r="EF1" s="2"/>
+      <c r="EG1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="EH1" s="1"/>
-      <c r="EI1" s="1" t="s">
+      <c r="EH1" s="2"/>
+      <c r="EI1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="EJ1" s="1"/>
-      <c r="EK1" s="1" t="s">
+      <c r="EJ1" s="2"/>
+      <c r="EK1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="EL1" s="1"/>
-      <c r="EM1" s="1" t="s">
+      <c r="EL1" s="2"/>
+      <c r="EM1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="EN1" s="1"/>
-      <c r="EO1" s="1" t="s">
+      <c r="EN1" s="2"/>
+      <c r="EO1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="EP1" s="1"/>
-      <c r="EQ1" s="1" t="s">
+      <c r="EP1" s="2"/>
+      <c r="EQ1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="ER1" s="1"/>
-      <c r="ES1" s="1" t="s">
+      <c r="ER1" s="2"/>
+      <c r="ES1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="ET1" s="1"/>
-      <c r="EU1" s="1" t="s">
+      <c r="ET1" s="2"/>
+      <c r="EU1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="EV1" s="1"/>
-      <c r="EW1" s="1" t="s">
+      <c r="EV1" s="2"/>
+      <c r="EW1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="EX1" s="1"/>
-      <c r="EY1" s="1" t="s">
+      <c r="EX1" s="2"/>
+      <c r="EY1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="EZ1" s="1"/>
-      <c r="FA1" s="1" t="s">
+      <c r="EZ1" s="2"/>
+      <c r="FA1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="FB1" s="1"/>
-      <c r="FC1" s="1" t="s">
+      <c r="FB1" s="2"/>
+      <c r="FC1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="FD1" s="1"/>
-      <c r="FE1" s="1" t="s">
+      <c r="FD1" s="2"/>
+      <c r="FE1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="FF1" s="1"/>
-      <c r="FG1" s="1" t="s">
+      <c r="FF1" s="2"/>
+      <c r="FG1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="FH1" s="1"/>
-      <c r="FI1" s="1" t="s">
+      <c r="FH1" s="2"/>
+      <c r="FI1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="FJ1" s="1"/>
-      <c r="FK1" s="1" t="s">
+      <c r="FJ1" s="2"/>
+      <c r="FK1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="FL1" s="1"/>
-      <c r="FM1" s="1" t="s">
+      <c r="FL1" s="2"/>
+      <c r="FM1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="FN1" s="1"/>
-      <c r="FO1" s="1"/>
-      <c r="FP1" s="1"/>
-      <c r="FQ1" s="1"/>
-      <c r="FR1" s="1"/>
-      <c r="FS1" s="1" t="s">
+      <c r="FN1" s="2"/>
+      <c r="FO1" s="2"/>
+      <c r="FP1" s="2"/>
+      <c r="FQ1" s="2"/>
+      <c r="FR1" s="2"/>
+      <c r="FS1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="FT1" s="1"/>
-      <c r="FU1" s="1"/>
-      <c r="FV1" s="1"/>
-      <c r="FW1" s="1"/>
+      <c r="FT1" s="2"/>
+      <c r="FU1" s="2"/>
+      <c r="FV1" s="2"/>
+      <c r="FW1" s="2"/>
     </row>
-    <row r="2" spans="1:179">
+    <row r="2" spans="1:179" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>53</v>
@@ -1261,28 +1316,28 @@
         <v>103</v>
       </c>
       <c r="BB2" s="1" t="s">
-        <v>104</v>
+        <v>140</v>
       </c>
       <c r="BC2" s="1" t="s">
-        <v>105</v>
+        <v>141</v>
       </c>
       <c r="BD2" s="1" t="s">
-        <v>106</v>
+        <v>142</v>
       </c>
       <c r="BE2" s="1" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="BF2" s="1" t="s">
-        <v>108</v>
+        <v>144</v>
       </c>
       <c r="BG2" s="1" t="s">
-        <v>109</v>
+        <v>145</v>
       </c>
       <c r="BH2" s="1" t="s">
         <v>100</v>
       </c>
       <c r="BI2" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="BJ2" s="1" t="s">
         <v>102</v>
@@ -1291,357 +1346,357 @@
         <v>103</v>
       </c>
       <c r="BL2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="BM2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="BN2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="BO2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="BP2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="BQ2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="BR2" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="BM2" s="1" t="s">
+      <c r="BS2" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="BN2" s="1" t="s">
+      <c r="BT2" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="BO2" s="1" t="s">
+      <c r="BU2" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="BP2" s="1" t="s">
+      <c r="BV2" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="BQ2" s="1" t="s">
+      <c r="BW2" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="BR2" s="1" t="s">
+      <c r="BX2" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="BS2" s="1" t="s">
+      <c r="BY2" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="BT2" s="1" t="s">
+      <c r="BZ2" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="BU2" s="1" t="s">
+      <c r="CA2" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="BV2" s="1" t="s">
+      <c r="CB2" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="BW2" s="1" t="s">
+      <c r="CC2" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="BX2" s="1" t="s">
+      <c r="CD2" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="BY2" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="BZ2" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="CA2" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="CB2" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="CC2" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="CD2" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="CE2" s="1" t="s">
         <v>90</v>
       </c>
       <c r="CF2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="CG2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="CH2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="CI2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="CJ2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="CK2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="CL2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="CM2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="CN2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="CO2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="CP2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="CQ2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="CR2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="CS2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="CT2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="CU2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="CV2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="CW2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="CX2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="CY2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="CZ2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="DA2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="DB2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="DC2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="DD2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="DE2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="DF2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="DG2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="DH2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="DI2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="DJ2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="DK2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="DL2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="DM2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="DN2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="DO2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="DP2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="DQ2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="DR2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="DS2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="DT2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="DU2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="DV2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="DW2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="DX2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="DY2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="DZ2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="EA2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="EB2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="EC2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="ED2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="EE2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="EF2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="EG2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="EH2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="EI2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="EJ2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="EK2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="EL2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="EM2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="EN2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="EO2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="EP2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="EQ2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="ER2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="ES2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="ET2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="EU2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="EV2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="EW2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="EX2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="EY2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="EZ2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="FA2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="FB2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="FC2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="FD2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="FE2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="FF2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="FG2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="FH2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="FI2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="FJ2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="FK2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="FL2" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="FM2" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="FN2" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="FO2" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="FP2" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="CG2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="CH2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="CI2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="CJ2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="CK2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="CL2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="CM2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="CN2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="CO2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="CP2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="CQ2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="CR2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="CS2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="CT2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="CU2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="CV2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="CW2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="CX2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="CY2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="CZ2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="DA2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="DB2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="DC2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="DD2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="DE2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="DF2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="DG2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="DH2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="DI2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="DJ2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="DK2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="DL2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="DM2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="DN2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="DO2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="DP2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="DQ2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="DR2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="DS2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="DT2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="DU2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="DV2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="DW2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="DX2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="DY2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="DZ2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="EA2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="EB2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="EC2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="ED2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="EE2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="EF2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="EG2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="EH2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="EI2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="EJ2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="EK2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="EL2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="EM2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="EN2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="EO2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="EP2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="EQ2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="ER2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="ES2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="ET2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="EU2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="EV2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="EW2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="EX2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="EY2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="EZ2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="FA2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="FB2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="FC2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="FD2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="FE2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="FF2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="FG2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="FH2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="FI2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="FJ2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="FK2" s="1" t="s">
+      <c r="FQ2" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="FL2" s="1" t="s">
+      <c r="FR2" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="FM2" s="1" t="s">
+      <c r="FS2" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="FN2" s="1" t="s">
+      <c r="FT2" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="FO2" s="1" t="s">
+      <c r="FU2" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="FP2" s="1" t="s">
+      <c r="FV2" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="FQ2" s="1" t="s">
+      <c r="FW2" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="FR2" s="1" t="s">
+    </row>
+    <row r="4" spans="1:179" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="FS2" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="FT2" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="FU2" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="FV2" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="FW2" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="4" spans="1:179">
-      <c r="A4" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="B4">
         <v>1.565466468583995</v>
@@ -1653,49 +1708,49 @@
         <v>0.3341095751237898</v>
       </c>
       <c r="E4">
-        <v>97.7627384468062</v>
+        <v>97.762738446806196</v>
       </c>
       <c r="F4">
-        <v>0.8799012220303121</v>
+        <v>0.87990122203031207</v>
       </c>
       <c r="G4">
-        <v>0.6881258160522931</v>
+        <v>0.68812581605229306</v>
       </c>
       <c r="H4">
-        <v>591.9444679083036</v>
+        <v>591.94446790830364</v>
       </c>
       <c r="I4">
-        <v>268.6419036434415</v>
+        <v>268.64190364344148</v>
       </c>
       <c r="J4">
         <v>228.6290029340845</v>
       </c>
       <c r="K4">
-        <v>343.7287217439676</v>
+        <v>343.72872174396758</v>
       </c>
       <c r="L4">
         <v>0</v>
       </c>
       <c r="M4">
-        <v>34.15368021512806</v>
+        <v>34.153680215128063</v>
       </c>
       <c r="N4">
-        <v>38.93370111310733</v>
+        <v>38.933701113107333</v>
       </c>
       <c r="O4">
-        <v>73.2930254420162</v>
+        <v>73.293025442016202</v>
       </c>
       <c r="P4">
-        <v>41.91213794307768</v>
+        <v>41.912137943077681</v>
       </c>
       <c r="Q4">
-        <v>2.692534576260401</v>
+        <v>2.6925345762604009</v>
       </c>
       <c r="R4">
-        <v>115.0688307888505</v>
+        <v>115.06883078885051</v>
       </c>
       <c r="S4">
-        <v>7.737752596246311</v>
+        <v>7.7377525962463114</v>
       </c>
       <c r="T4">
         <v>12.93966370498595</v>
@@ -1704,64 +1759,64 @@
         <v>0</v>
       </c>
       <c r="V4">
-        <v>9.332506447044631</v>
+        <v>9.3325064470446311</v>
       </c>
       <c r="W4">
-        <v>2.150459790011743</v>
+        <v>2.1504597900117428</v>
       </c>
       <c r="X4">
         <v>51.64975189962</v>
       </c>
       <c r="Y4">
-        <v>0.2612653460101035</v>
+        <v>0.26126534601010348</v>
       </c>
       <c r="Z4">
-        <v>62.11660282668066</v>
+        <v>62.116602826680662</v>
       </c>
       <c r="AA4">
-        <v>0.09779069781481038</v>
+        <v>9.7790697814810382E-2</v>
       </c>
       <c r="AB4">
-        <v>39.6280544730793</v>
+        <v>39.628054473079303</v>
       </c>
       <c r="AC4">
         <v>27.93535241569634</v>
       </c>
       <c r="AD4">
-        <v>21.32892647329602</v>
+        <v>21.328926473296018</v>
       </c>
       <c r="AE4">
-        <v>0.4110336246538933</v>
+        <v>0.41103362465389331</v>
       </c>
       <c r="AF4">
-        <v>0.03965119174252279</v>
+        <v>3.9651191742522789E-2</v>
       </c>
       <c r="AG4">
-        <v>2.884011194898403</v>
+        <v>2.8840111948984029</v>
       </c>
       <c r="AH4">
-        <v>5.805051431937406</v>
+        <v>5.8050514319374056</v>
       </c>
       <c r="AI4">
-        <v>0.3155667752997641</v>
+        <v>0.31556677529976412</v>
       </c>
       <c r="AJ4">
         <v>1.284520453895988</v>
       </c>
       <c r="AK4">
-        <v>0.06941155863178289</v>
+        <v>6.9411558631782888E-2</v>
       </c>
       <c r="AL4">
-        <v>0.0507457502263939</v>
+        <v>5.0745750226393903E-2</v>
       </c>
       <c r="AM4">
-        <v>2.842170943040401E-14</v>
+        <v>2.8421709430404007E-14</v>
       </c>
       <c r="AN4">
-        <v>343.7287217439676</v>
+        <v>343.72872174396758</v>
       </c>
       <c r="AO4">
-        <v>-3.388457892402866</v>
+        <v>-3.3884578924028661</v>
       </c>
       <c r="AP4">
         <v>0</v>
@@ -1776,7 +1831,7 @@
         <v>0</v>
       </c>
       <c r="AT4">
-        <v>1968.739338615159</v>
+        <v>1968.7393386151591</v>
       </c>
       <c r="AU4">
         <v>0</v>
@@ -1797,13 +1852,13 @@
         <v>1883.313578069911</v>
       </c>
       <c r="BA4">
-        <v>2.273736754432321E-13</v>
+        <v>2.2737367544323211E-13</v>
       </c>
       <c r="BB4">
-        <v>-62.71767829121965</v>
+        <v>-62.717678291219649</v>
       </c>
       <c r="BC4">
-        <v>-37.87222141372013</v>
+        <v>-37.872221413720133</v>
       </c>
       <c r="BD4">
         <v>-1797.535036639762</v>
@@ -1812,28 +1867,28 @@
         <v>-110.4202740612708</v>
       </c>
       <c r="BF4">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BG4">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BH4">
-        <v>291.8902551818514</v>
+        <v>291.89025518185139</v>
       </c>
       <c r="BI4">
-        <v>1716.654955224121</v>
+        <v>1716.6549552241211</v>
       </c>
       <c r="BJ4">
-        <v>-1716.654955224121</v>
+        <v>-1716.6549552241211</v>
       </c>
       <c r="BK4">
-        <v>-2.273736754432321E-13</v>
+        <v>-2.2737367544323211E-13</v>
       </c>
       <c r="BL4">
-        <v>6114.211142072342</v>
+        <v>6114.2111420723422</v>
       </c>
       <c r="BM4">
-        <v>693.2881528751886</v>
+        <v>693.28815287518864</v>
       </c>
       <c r="BN4">
         <v>11702.44575894857</v>
@@ -1845,61 +1900,61 @@
         <v>0</v>
       </c>
       <c r="BQ4">
-        <v>10469.00177855886</v>
+        <v>10469.001778558861</v>
       </c>
       <c r="BR4">
-        <v>7194.316157218206</v>
+        <v>7194.3161572182062</v>
       </c>
       <c r="BS4">
-        <v>469.373897743323</v>
+        <v>469.37389774332303</v>
       </c>
       <c r="BT4">
-        <v>46332.45549850338</v>
+        <v>46332.455498503383</v>
       </c>
       <c r="BU4">
         <v>0</v>
       </c>
       <c r="BV4">
-        <v>3.374310845086885</v>
+        <v>3.3743108450868848</v>
       </c>
       <c r="BW4">
-        <v>0.3826118658087591</v>
+        <v>0.38261186580875911</v>
       </c>
       <c r="BX4">
-        <v>6.458345765448535</v>
+        <v>6.4583457654485352</v>
       </c>
       <c r="BY4">
-        <v>5.34761709508664</v>
+        <v>5.3476170950866404</v>
       </c>
       <c r="BZ4">
         <v>0</v>
       </c>
       <c r="CA4">
-        <v>5.777632701551065</v>
+        <v>5.7776327015510649</v>
       </c>
       <c r="CB4">
-        <v>3.970399200845584</v>
+        <v>3.9703992008455842</v>
       </c>
       <c r="CC4">
-        <v>0.2590380666865852</v>
+        <v>0.25903806668658519</v>
       </c>
       <c r="CD4">
-        <v>25.56995554051405</v>
+        <v>25.569955540514052</v>
       </c>
       <c r="CE4">
-        <v>3.552713678800501E-15</v>
+        <v>3.5527136788005009E-15</v>
       </c>
       <c r="CF4">
-        <v>-943.7062939880416</v>
+        <v>-943.70629398804158</v>
       </c>
       <c r="CG4">
-        <v>1.354136264957409</v>
+        <v>1.3541362649574089</v>
       </c>
       <c r="CH4">
         <v>-109.3166444227099</v>
       </c>
       <c r="CI4">
-        <v>1.372175149794833</v>
+        <v>1.3721751497948329</v>
       </c>
       <c r="CJ4">
         <v>-142.9704675972462</v>
@@ -1911,25 +1966,25 @@
         <v>-183.8727593161166</v>
       </c>
       <c r="CM4">
-        <v>1.410718671247078</v>
+        <v>1.4107186712470781</v>
       </c>
       <c r="CN4">
-        <v>-232.6969573162496</v>
+        <v>-232.69695731624961</v>
       </c>
       <c r="CO4">
         <v>1.431028535706018</v>
       </c>
       <c r="CP4">
-        <v>-292.9559457749128</v>
+        <v>-292.95594577491278</v>
       </c>
       <c r="CQ4">
-        <v>1.452092558065024</v>
+        <v>1.4520925580650239</v>
       </c>
       <c r="CR4">
-        <v>-363.1606647912413</v>
+        <v>-363.16066479124129</v>
       </c>
       <c r="CS4">
-        <v>1.473634337684271</v>
+        <v>1.4736343376842711</v>
       </c>
       <c r="CT4">
         <v>-440.3204189427197</v>
@@ -1938,34 +1993,34 @@
         <v>1.495753672724015</v>
       </c>
       <c r="CV4">
-        <v>-538.9597185067832</v>
+        <v>-538.95971850678325</v>
       </c>
       <c r="CW4">
         <v>1.518265016315661</v>
       </c>
       <c r="CX4">
-        <v>-637.9901691330597</v>
+        <v>-637.99016913305968</v>
       </c>
       <c r="CY4">
         <v>1.541450805796249</v>
       </c>
       <c r="CZ4">
-        <v>-809.2295061619952</v>
+        <v>-809.22950616199523</v>
       </c>
       <c r="DA4">
-        <v>1.589991970999519</v>
+        <v>1.5899919709995189</v>
       </c>
       <c r="DB4">
-        <v>-1127.279785392806</v>
+        <v>-1127.2797853928059</v>
       </c>
       <c r="DC4">
-        <v>1.614900548335472</v>
+        <v>1.6149005483354719</v>
       </c>
       <c r="DD4">
-        <v>-1288.240133698098</v>
+        <v>-1288.2401336980979</v>
       </c>
       <c r="DE4">
-        <v>1.640195969043173</v>
+        <v>1.6401959690431731</v>
       </c>
       <c r="DF4">
         <v>-1464.012125710025</v>
@@ -1974,31 +2029,31 @@
         <v>1.666340245047881</v>
       </c>
       <c r="DH4">
-        <v>-1616.650812880369</v>
+        <v>-1616.6508128803689</v>
       </c>
       <c r="DI4">
         <v>1.692666146407104</v>
       </c>
       <c r="DJ4">
-        <v>-1715.998097892851</v>
+        <v>-1715.9980978928511</v>
       </c>
       <c r="DK4">
-        <v>1.719441808777369</v>
+        <v>1.7194418087773691</v>
       </c>
       <c r="DL4">
-        <v>-1899.823512604227</v>
+        <v>-1899.8235126042271</v>
       </c>
       <c r="DM4">
-        <v>1.747761049152419</v>
+        <v>1.7477610491524189</v>
       </c>
       <c r="DN4">
-        <v>-1372.394358293852</v>
+        <v>-1372.3943582938521</v>
       </c>
       <c r="DO4">
-        <v>1.776508141716982</v>
+        <v>1.7765081417169819</v>
       </c>
       <c r="DP4">
-        <v>-1518.918316913419</v>
+        <v>-1518.9183169134189</v>
       </c>
       <c r="DQ4">
         <v>1.805545270647454</v>
@@ -2016,10 +2071,10 @@
         <v>1.864471009336041</v>
       </c>
       <c r="DV4">
-        <v>-2000.02310850122</v>
+        <v>-2000.0231085012199</v>
       </c>
       <c r="DW4">
-        <v>1.894356347019324</v>
+        <v>1.8943563470193241</v>
       </c>
       <c r="DX4">
         <v>-2173.587656844466</v>
@@ -2028,7 +2083,7 @@
         <v>1.924524161259805</v>
       </c>
       <c r="DZ4">
-        <v>-2353.448734172853</v>
+        <v>-2353.4487341728532</v>
       </c>
       <c r="EA4">
         <v>1.954976711656111</v>
@@ -2037,52 +2092,52 @@
         <v>-2539.434215216927</v>
       </c>
       <c r="EC4">
-        <v>1.985717168000661</v>
+        <v>1.9857171680006609</v>
       </c>
       <c r="ED4">
-        <v>-2731.38764194565</v>
+        <v>-2731.3876419456501</v>
       </c>
       <c r="EE4">
-        <v>2.016749349608861</v>
+        <v>2.0167493496088609</v>
       </c>
       <c r="EF4">
         <v>-2929.158220557787</v>
       </c>
       <c r="EG4">
-        <v>2.048077516337364</v>
+        <v>2.0480775163373641</v>
       </c>
       <c r="EH4">
         <v>-3132.608726028207</v>
       </c>
       <c r="EI4">
-        <v>2.079706203306247</v>
+        <v>2.0797062033062468</v>
       </c>
       <c r="EJ4">
-        <v>-3341.606252934391</v>
+        <v>-3341.6062529343908</v>
       </c>
       <c r="EK4">
-        <v>2.111640091981443</v>
+        <v>2.1116400919814429</v>
       </c>
       <c r="EL4">
         <v>-3556.028300444174</v>
       </c>
       <c r="EM4">
-        <v>2.143883911205592</v>
+        <v>2.1438839112055921</v>
       </c>
       <c r="EN4">
         <v>-3775.76290301769</v>
       </c>
       <c r="EO4">
-        <v>2.17644236261178</v>
+        <v>2.1764423626117799</v>
       </c>
       <c r="EP4">
-        <v>-4000.700599542659</v>
+        <v>-4000.7005995426589</v>
       </c>
       <c r="EQ4">
         <v>2.209320065637383</v>
       </c>
       <c r="ER4">
-        <v>-4230.743257438182</v>
+        <v>-4230.7432574381819</v>
       </c>
       <c r="ES4">
         <v>2.242521518225344</v>
@@ -2091,117 +2146,117 @@
         <v>-4465.794614604114</v>
       </c>
       <c r="EU4">
-        <v>2.276051069851282</v>
+        <v>2.2760510698512819</v>
       </c>
       <c r="EV4">
-        <v>-4705.769189146158</v>
+        <v>-4705.7691891461582</v>
       </c>
       <c r="EW4">
-        <v>2.309912904242923</v>
+        <v>2.3099129042429229</v>
       </c>
       <c r="EX4">
-        <v>-4950.581768426782</v>
+        <v>-4950.5817684267822</v>
       </c>
       <c r="EY4">
-        <v>2.344111029520371</v>
+        <v>2.3441110295203709</v>
       </c>
       <c r="EZ4">
-        <v>-5200.154661563622</v>
+        <v>-5200.1546615636216</v>
       </c>
       <c r="FA4">
         <v>2.378649274037858</v>
       </c>
       <c r="FB4">
-        <v>-5454.414143487895</v>
+        <v>-5454.4141434878948</v>
       </c>
       <c r="FC4">
-        <v>2.41353128647933</v>
+        <v>2.4135312864793299</v>
       </c>
       <c r="FD4">
-        <v>-5713.289947568497</v>
+        <v>-5713.2899475684972</v>
       </c>
       <c r="FE4">
-        <v>2.44876053908153</v>
+        <v>2.4487605390815301</v>
       </c>
       <c r="FF4">
-        <v>-5976.716186621517</v>
+        <v>-5976.7161866215174</v>
       </c>
       <c r="FG4">
-        <v>2.484340333103011</v>
+        <v>2.4843403331030109</v>
       </c>
       <c r="FH4">
-        <v>-6244.629967563431</v>
+        <v>-6244.6299675634309</v>
       </c>
       <c r="FI4">
         <v>1.565466468583995</v>
       </c>
       <c r="FJ4">
-        <v>-943.7062939880416</v>
+        <v>-943.70629398804158</v>
       </c>
       <c r="FK4">
-        <v>5.919347097929955</v>
+        <v>5.9193470979299549</v>
       </c>
       <c r="FL4">
-        <v>77.18228942343981</v>
+        <v>77.182289423439812</v>
       </c>
       <c r="FM4">
-        <v>0.7985481666807733</v>
+        <v>0.79854816668077333</v>
       </c>
       <c r="FN4">
-        <v>0.4472755030905158</v>
+        <v>0.44727550309051578</v>
       </c>
       <c r="FO4">
-        <v>3.067542517366735</v>
+        <v>3.0675425173667352</v>
       </c>
       <c r="FP4">
-        <v>0.9174305109602631</v>
+        <v>0.91743051096026307</v>
       </c>
       <c r="FQ4">
-        <v>0.6885503998316683</v>
+        <v>0.68855039983166832</v>
       </c>
       <c r="FR4">
-        <v>-3.33066907387547E-16</v>
+        <v>-3.3306690738754701E-16</v>
       </c>
       <c r="FS4">
         <v>9.858742574479713</v>
       </c>
       <c r="FT4">
-        <v>55.90943788631447</v>
+        <v>55.909437886314471</v>
       </c>
       <c r="FU4">
         <v>3.481968822993371</v>
       </c>
       <c r="FV4">
-        <v>7.93214013965225</v>
+        <v>7.9321401396522502</v>
       </c>
       <c r="FW4">
-        <v>7.105427357601002E-15</v>
+        <v>7.1054273576010019E-15</v>
       </c>
     </row>
-    <row r="5" spans="1:179">
+    <row r="5" spans="1:179" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B5">
-        <v>1.564913376272287</v>
+        <v>1.5649133762722871</v>
       </c>
       <c r="C5">
-        <v>219.6497966146568</v>
+        <v>219.64979661465679</v>
       </c>
       <c r="D5">
-        <v>0.3342317279823218</v>
+        <v>0.33423172798232181</v>
       </c>
       <c r="E5">
-        <v>97.79265706011029</v>
+        <v>97.792657060110287</v>
       </c>
       <c r="F5">
-        <v>0.8799032113965172</v>
+        <v>0.87990321139651717</v>
       </c>
       <c r="G5">
-        <v>0.6881640187484345</v>
+        <v>0.68816401874843447</v>
       </c>
       <c r="H5">
-        <v>591.7052957261276</v>
+        <v>591.70529572612759</v>
       </c>
       <c r="I5">
         <v>268.6755292627148</v>
@@ -2210,106 +2265,106 @@
         <v>228.6636886761801</v>
       </c>
       <c r="K5">
-        <v>343.7329048177637</v>
+        <v>343.73290481776371</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5">
-        <v>34.15368051092405</v>
+        <v>34.153680510924048</v>
       </c>
       <c r="N5">
-        <v>38.7870016741013</v>
+        <v>38.787001674101298</v>
       </c>
       <c r="O5">
-        <v>73.30789343723637</v>
+        <v>73.307893437236373</v>
       </c>
       <c r="P5">
-        <v>41.91212418762876</v>
+        <v>41.912124187628763</v>
       </c>
       <c r="Q5">
-        <v>2.692981239189474</v>
+        <v>2.6929812391894741</v>
       </c>
       <c r="R5">
-        <v>115.0772687926953</v>
+        <v>115.07726879269531</v>
       </c>
       <c r="S5">
-        <v>7.739571289906667</v>
+        <v>7.7395712899066673</v>
       </c>
       <c r="T5">
         <v>12.94151130473624</v>
       </c>
       <c r="U5">
-        <v>-5.684341886080801E-14</v>
+        <v>-5.6843418860808009E-14</v>
       </c>
       <c r="V5">
-        <v>9.332506447044631</v>
+        <v>9.3325064470446311</v>
       </c>
       <c r="W5">
-        <v>2.15045969282537</v>
+        <v>2.1504596928253701</v>
       </c>
       <c r="X5">
         <v>51.64975189962</v>
       </c>
       <c r="Y5">
-        <v>0.2613570201362548</v>
+        <v>0.26135702013625478</v>
       </c>
       <c r="Z5">
-        <v>62.13290969768557</v>
+        <v>62.132909697685569</v>
       </c>
       <c r="AA5">
-        <v>0.09779075484059006</v>
+        <v>9.7790754840590063E-2</v>
       </c>
       <c r="AB5">
-        <v>39.63988302268952</v>
+        <v>39.639883022689517</v>
       </c>
       <c r="AC5">
         <v>27.93535241569634</v>
       </c>
       <c r="AD5">
-        <v>21.33480422175529</v>
+        <v>21.334804221755292</v>
       </c>
       <c r="AE5">
-        <v>0.411131593729619</v>
+        <v>0.41113159372961899</v>
       </c>
       <c r="AF5">
-        <v>0.03965615018214547</v>
+        <v>3.9656150182145473E-2</v>
       </c>
       <c r="AG5">
         <v>2.885117577819281</v>
       </c>
       <c r="AH5">
-        <v>5.805051431937406</v>
+        <v>5.8050514319374056</v>
       </c>
       <c r="AI5">
-        <v>0.3156062373873705</v>
+        <v>0.31560623738737048</v>
       </c>
       <c r="AJ5">
         <v>1.283499098095729</v>
       </c>
       <c r="AK5">
-        <v>0.06939243571518319</v>
+        <v>6.9392435715183193E-2</v>
       </c>
       <c r="AL5">
-        <v>0.05073176974866805</v>
+        <v>5.0731769748668047E-2</v>
       </c>
       <c r="AM5">
-        <v>-8.526512829121202E-14</v>
+        <v>-8.5265128291212022E-14</v>
       </c>
       <c r="AN5">
-        <v>343.7329048177637</v>
+        <v>343.73290481776371</v>
       </c>
       <c r="AO5">
-        <v>-3.388811414734931</v>
+        <v>-3.3888114147349309</v>
       </c>
       <c r="AP5">
         <v>0</v>
       </c>
       <c r="AQ5">
-        <v>5.684341886080801E-14</v>
+        <v>5.6843418860808009E-14</v>
       </c>
       <c r="AR5">
-        <v>150.4248052763016</v>
+        <v>150.42480527630161</v>
       </c>
       <c r="AS5">
         <v>0</v>
@@ -2330,70 +2385,70 @@
         <v>-235.8917941266341</v>
       </c>
       <c r="AY5">
-        <v>-1883.549089192201</v>
+        <v>-1883.5490891922011</v>
       </c>
       <c r="AZ5">
-        <v>1883.549089192201</v>
+        <v>1883.5490891922011</v>
       </c>
       <c r="BA5">
-        <v>2.273736754432321E-13</v>
+        <v>2.2737367544323211E-13</v>
       </c>
       <c r="BB5">
-        <v>-62.71795660034657</v>
+        <v>-62.717956600346568</v>
       </c>
       <c r="BC5">
         <v>-37.87001970223271</v>
       </c>
       <c r="BD5">
-        <v>-1797.815667090768</v>
+        <v>-1797.8156670907681</v>
       </c>
       <c r="BE5">
         <v>-110.4183767261715</v>
       </c>
       <c r="BF5">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BG5">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BH5">
-        <v>291.5647161900416</v>
+        <v>291.56471619004162</v>
       </c>
       <c r="BI5">
-        <v>1717.257303929477</v>
+        <v>1717.2573039294771</v>
       </c>
       <c r="BJ5">
-        <v>-1717.257303929477</v>
+        <v>-1717.2573039294771</v>
       </c>
       <c r="BK5">
         <v>0</v>
       </c>
       <c r="BL5">
-        <v>6114.210788272152</v>
+        <v>6114.2107882721521</v>
       </c>
       <c r="BM5">
-        <v>691.7031665868354</v>
+        <v>691.70316658683544</v>
       </c>
       <c r="BN5">
         <v>11708.31128496306</v>
       </c>
       <c r="BO5">
-        <v>9689.816876699411</v>
+        <v>9689.8168766994113</v>
       </c>
       <c r="BP5">
         <v>0</v>
       </c>
       <c r="BQ5">
-        <v>10470.28208520502</v>
+        <v>10470.282085205021</v>
       </c>
       <c r="BR5">
-        <v>7196.840535812769</v>
+        <v>7196.8405358127693</v>
       </c>
       <c r="BS5">
-        <v>469.4253062128049</v>
+        <v>469.42530621280491</v>
       </c>
       <c r="BT5">
-        <v>46340.59004375205</v>
+        <v>46340.590043752047</v>
       </c>
       <c r="BU5">
         <v>0</v>
@@ -2402,34 +2457,34 @@
         <v>3.374310649831636</v>
       </c>
       <c r="BW5">
-        <v>0.3817371435759427</v>
+        <v>0.38173714357594268</v>
       </c>
       <c r="BX5">
-        <v>6.461582831945414</v>
+        <v>6.4615828319454138</v>
       </c>
       <c r="BY5">
-        <v>5.347616137912873</v>
+        <v>5.3476161379128726</v>
       </c>
       <c r="BZ5">
         <v>0</v>
       </c>
       <c r="CA5">
-        <v>5.778339277182946</v>
+        <v>5.7783392771829458</v>
       </c>
       <c r="CB5">
-        <v>3.971792354904352</v>
+        <v>3.9717923549043519</v>
       </c>
       <c r="CC5">
-        <v>0.2590664379927228</v>
+        <v>0.25906643799272278</v>
       </c>
       <c r="CD5">
         <v>25.57444483334589</v>
       </c>
       <c r="CE5">
-        <v>-3.552713678800501E-15</v>
+        <v>-3.5527136788005009E-15</v>
       </c>
       <c r="CF5">
-        <v>-943.7177786938846</v>
+        <v>-943.71777869388461</v>
       </c>
       <c r="CG5">
         <v>1.353742286587321</v>
@@ -2447,73 +2502,73 @@
         <v>1.390647055057048</v>
       </c>
       <c r="CL5">
-        <v>-183.8828792124987</v>
+        <v>-183.88287921249869</v>
       </c>
       <c r="CM5">
-        <v>1.410281921256831</v>
+        <v>1.4102819212568309</v>
       </c>
       <c r="CN5">
-        <v>-232.7113826796412</v>
+        <v>-232.71138267964119</v>
       </c>
       <c r="CO5">
         <v>1.430576357831836</v>
       </c>
       <c r="CP5">
-        <v>-292.9647406563163</v>
+        <v>-292.96474065631628</v>
       </c>
       <c r="CQ5">
         <v>1.451624475581762</v>
       </c>
       <c r="CR5">
-        <v>-363.1759476270527</v>
+        <v>-363.17594762705272</v>
       </c>
       <c r="CS5">
         <v>1.473149993954078</v>
       </c>
       <c r="CT5">
-        <v>-440.3366299401969</v>
+        <v>-440.33662994019687</v>
       </c>
       <c r="CU5">
         <v>1.495252658041424</v>
       </c>
       <c r="CV5">
-        <v>-538.9750929661095</v>
+        <v>-538.97509296610951</v>
       </c>
       <c r="CW5">
-        <v>1.517747013296925</v>
+        <v>1.5177470132969251</v>
       </c>
       <c r="CX5">
-        <v>-638.0051736291498</v>
+        <v>-638.00517362914979</v>
       </c>
       <c r="CY5">
         <v>1.540915823472232</v>
       </c>
       <c r="CZ5">
-        <v>-809.2562778163701</v>
+        <v>-809.25627781637013</v>
       </c>
       <c r="DA5">
-        <v>1.589420756558415</v>
+        <v>1.5894207565584151</v>
       </c>
       <c r="DB5">
-        <v>-1127.287969052326</v>
+        <v>-1127.2879690523259</v>
       </c>
       <c r="DC5">
-        <v>1.614310555701088</v>
+        <v>1.6143105557010879</v>
       </c>
       <c r="DD5">
-        <v>-1288.24009754369</v>
+        <v>-1288.2400975436899</v>
       </c>
       <c r="DE5">
-        <v>1.639587658789366</v>
+        <v>1.6395876587893661</v>
       </c>
       <c r="DF5">
-        <v>-1464.011977144051</v>
+        <v>-1464.0119771440509</v>
       </c>
       <c r="DG5">
-        <v>1.665711063299348</v>
+        <v>1.6657110632993479</v>
       </c>
       <c r="DH5">
-        <v>-1616.59360805992</v>
+        <v>-1616.5936080599199</v>
       </c>
       <c r="DI5">
         <v>1.692017143351227</v>
@@ -2525,22 +2580,22 @@
         <v>1.718774197328653</v>
       </c>
       <c r="DL5">
-        <v>-1899.991634689737</v>
+        <v>-1899.9916346897371</v>
       </c>
       <c r="DM5">
         <v>1.747071902240533</v>
       </c>
       <c r="DN5">
-        <v>-1372.353592069121</v>
+        <v>-1372.3535920691211</v>
       </c>
       <c r="DO5">
-        <v>1.775797374723974</v>
+        <v>1.7757973747239739</v>
       </c>
       <c r="DP5">
         <v>-1518.865443046903</v>
       </c>
       <c r="DQ5">
-        <v>1.804812653009754</v>
+        <v>1.8048126530097539</v>
       </c>
       <c r="DR5">
         <v>-1672.429629136692</v>
@@ -2549,10 +2604,10 @@
         <v>1.834112424392089</v>
       </c>
       <c r="DT5">
-        <v>-1832.846640907694</v>
+        <v>-1832.8466409076941</v>
       </c>
       <c r="DU5">
-        <v>1.863694010806504</v>
+        <v>1.8636940108065041</v>
       </c>
       <c r="DV5">
         <v>-1999.920332802518</v>
@@ -2561,13 +2616,13 @@
         <v>1.893556819997575</v>
       </c>
       <c r="DX5">
-        <v>-2173.465533477138</v>
+        <v>-2173.4655334771378</v>
       </c>
       <c r="DY5">
-        <v>1.923701879438431</v>
+        <v>1.9237018794384311</v>
       </c>
       <c r="DZ5">
-        <v>-2353.302854096866</v>
+        <v>-2353.3028540968662</v>
       </c>
       <c r="EA5">
         <v>1.954131446871086</v>
@@ -2579,10 +2634,10 @@
         <v>1.984848689613933</v>
       </c>
       <c r="ED5">
-        <v>-2731.191308123205</v>
+        <v>-2731.1913081232051</v>
       </c>
       <c r="EE5">
-        <v>2.015857424064306</v>
+        <v>2.0158574240643059</v>
       </c>
       <c r="EF5">
         <v>-2928.934596020059</v>
@@ -2591,31 +2646,31 @@
         <v>2.047161906880882</v>
       </c>
       <c r="EH5">
-        <v>-3132.351714948367</v>
+        <v>-3132.3517149483669</v>
       </c>
       <c r="EI5">
-        <v>2.078766669792386</v>
+        <v>2.0787666697923859</v>
       </c>
       <c r="EJ5">
         <v>-3341.317484599334</v>
       </c>
       <c r="EK5">
-        <v>2.110676390808741</v>
+        <v>2.1106763908087411</v>
       </c>
       <c r="EL5">
-        <v>-3555.705726156477</v>
+        <v>-3555.7057261564769</v>
       </c>
       <c r="EM5">
-        <v>2.142895795302841</v>
+        <v>2.1428957953028411</v>
       </c>
       <c r="EN5">
-        <v>-3775.401549231916</v>
+        <v>-3775.4015492319159</v>
       </c>
       <c r="EO5">
         <v>2.175429581461382</v>
       </c>
       <c r="EP5">
-        <v>-4000.301069618639</v>
+        <v>-4000.3010696186388</v>
       </c>
       <c r="EQ5">
         <v>2.208282365369453</v>
@@ -2627,150 +2682,150 @@
         <v>2.241458641704706</v>
       </c>
       <c r="ET5">
-        <v>-4465.309881976675</v>
+        <v>-4465.3098819766747</v>
       </c>
       <c r="EU5">
-        <v>2.274962756807776</v>
+        <v>2.2749627568077759</v>
       </c>
       <c r="EV5">
-        <v>-4705.238909773889</v>
+        <v>-4705.2389097738887</v>
       </c>
       <c r="EW5">
         <v>2.308798891397899</v>
       </c>
       <c r="EX5">
-        <v>-4950.003341598309</v>
+        <v>-4950.0033415983089</v>
       </c>
       <c r="EY5">
-        <v>2.342971050722346</v>
+        <v>2.3429710507223458</v>
       </c>
       <c r="EZ5">
-        <v>-5199.525684213982</v>
+        <v>-5199.5256842139815</v>
       </c>
       <c r="FA5">
-        <v>2.377483060398146</v>
+        <v>2.3774830603981458</v>
       </c>
       <c r="FB5">
-        <v>-5453.733250502301</v>
+        <v>-5453.7332505023014</v>
       </c>
       <c r="FC5">
         <v>2.412338566512247</v>
       </c>
       <c r="FD5">
-        <v>-5712.554912381833</v>
+        <v>-5712.5549123818328</v>
       </c>
       <c r="FE5">
         <v>2.447541038838478</v>
       </c>
       <c r="FF5">
-        <v>-5975.923402039076</v>
+        <v>-5975.9234020390759</v>
       </c>
       <c r="FG5">
-        <v>2.483093776290766</v>
+        <v>2.4830937762907661</v>
       </c>
       <c r="FH5">
-        <v>-6243.778510524446</v>
+        <v>-6243.7785105244457</v>
       </c>
       <c r="FI5">
-        <v>1.564913376272287</v>
+        <v>1.5649133762722871</v>
       </c>
       <c r="FJ5">
-        <v>-943.7177786938846</v>
+        <v>-943.71777869388461</v>
       </c>
       <c r="FK5">
-        <v>5.918523000449707</v>
+        <v>5.9185230004497074</v>
       </c>
       <c r="FL5">
-        <v>77.17166132546311</v>
+        <v>77.171661325463106</v>
       </c>
       <c r="FM5">
-        <v>0.7983964675461476</v>
+        <v>0.79839646754614757</v>
       </c>
       <c r="FN5">
-        <v>0.4472294117200613</v>
+        <v>0.44722941172006131</v>
       </c>
       <c r="FO5">
-        <v>3.067226409648838</v>
+        <v>3.0672264096488382</v>
       </c>
       <c r="FP5">
-        <v>0.9173374681430704</v>
+        <v>0.91733746814307038</v>
       </c>
       <c r="FQ5">
-        <v>0.6883332433915896</v>
+        <v>0.68833324339158963</v>
       </c>
       <c r="FR5">
-        <v>7.424616477180734E-16</v>
+        <v>7.4246164771807344E-16</v>
       </c>
       <c r="FS5">
-        <v>9.856869722246813</v>
+        <v>9.8568697222468131</v>
       </c>
       <c r="FT5">
-        <v>55.90367646500765</v>
+        <v>55.903676465007649</v>
       </c>
       <c r="FU5">
         <v>3.481615693045327</v>
       </c>
       <c r="FV5">
-        <v>7.929499445163316</v>
+        <v>7.9294994451633158</v>
       </c>
       <c r="FW5">
-        <v>-1.77635683940025E-15</v>
+        <v>-1.7763568394002501E-15</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="52">
+    <mergeCell ref="FM1:FR1"/>
+    <mergeCell ref="FS1:FW1"/>
+    <mergeCell ref="FC1:FD1"/>
+    <mergeCell ref="FE1:FF1"/>
+    <mergeCell ref="FG1:FH1"/>
+    <mergeCell ref="FI1:FJ1"/>
+    <mergeCell ref="FK1:FL1"/>
+    <mergeCell ref="ES1:ET1"/>
+    <mergeCell ref="EU1:EV1"/>
+    <mergeCell ref="EW1:EX1"/>
+    <mergeCell ref="EY1:EZ1"/>
+    <mergeCell ref="FA1:FB1"/>
+    <mergeCell ref="EI1:EJ1"/>
+    <mergeCell ref="EK1:EL1"/>
+    <mergeCell ref="EM1:EN1"/>
+    <mergeCell ref="EO1:EP1"/>
+    <mergeCell ref="EQ1:ER1"/>
+    <mergeCell ref="DY1:DZ1"/>
+    <mergeCell ref="EA1:EB1"/>
+    <mergeCell ref="EC1:ED1"/>
+    <mergeCell ref="EE1:EF1"/>
+    <mergeCell ref="EG1:EH1"/>
+    <mergeCell ref="DO1:DP1"/>
+    <mergeCell ref="DQ1:DR1"/>
+    <mergeCell ref="DS1:DT1"/>
+    <mergeCell ref="DU1:DV1"/>
+    <mergeCell ref="DW1:DX1"/>
+    <mergeCell ref="DE1:DF1"/>
+    <mergeCell ref="DG1:DH1"/>
+    <mergeCell ref="DI1:DJ1"/>
+    <mergeCell ref="DK1:DL1"/>
+    <mergeCell ref="DM1:DN1"/>
+    <mergeCell ref="CU1:CV1"/>
+    <mergeCell ref="CW1:CX1"/>
+    <mergeCell ref="CY1:CZ1"/>
+    <mergeCell ref="DA1:DB1"/>
+    <mergeCell ref="DC1:DD1"/>
+    <mergeCell ref="CK1:CL1"/>
+    <mergeCell ref="CM1:CN1"/>
+    <mergeCell ref="CO1:CP1"/>
+    <mergeCell ref="CQ1:CR1"/>
+    <mergeCell ref="CS1:CT1"/>
+    <mergeCell ref="BB1:BK1"/>
+    <mergeCell ref="BL1:BU1"/>
+    <mergeCell ref="BV1:CE1"/>
+    <mergeCell ref="CG1:CH1"/>
+    <mergeCell ref="CI1:CJ1"/>
     <mergeCell ref="B1:L1"/>
     <mergeCell ref="M1:U1"/>
     <mergeCell ref="V1:AM1"/>
     <mergeCell ref="AN1:AQ1"/>
     <mergeCell ref="AR1:BA1"/>
-    <mergeCell ref="BB1:BK1"/>
-    <mergeCell ref="BL1:BU1"/>
-    <mergeCell ref="BV1:CE1"/>
-    <mergeCell ref="CG1:CH1"/>
-    <mergeCell ref="CI1:CJ1"/>
-    <mergeCell ref="CK1:CL1"/>
-    <mergeCell ref="CM1:CN1"/>
-    <mergeCell ref="CO1:CP1"/>
-    <mergeCell ref="CQ1:CR1"/>
-    <mergeCell ref="CS1:CT1"/>
-    <mergeCell ref="CU1:CV1"/>
-    <mergeCell ref="CW1:CX1"/>
-    <mergeCell ref="CY1:CZ1"/>
-    <mergeCell ref="DA1:DB1"/>
-    <mergeCell ref="DC1:DD1"/>
-    <mergeCell ref="DE1:DF1"/>
-    <mergeCell ref="DG1:DH1"/>
-    <mergeCell ref="DI1:DJ1"/>
-    <mergeCell ref="DK1:DL1"/>
-    <mergeCell ref="DM1:DN1"/>
-    <mergeCell ref="DO1:DP1"/>
-    <mergeCell ref="DQ1:DR1"/>
-    <mergeCell ref="DS1:DT1"/>
-    <mergeCell ref="DU1:DV1"/>
-    <mergeCell ref="DW1:DX1"/>
-    <mergeCell ref="DY1:DZ1"/>
-    <mergeCell ref="EA1:EB1"/>
-    <mergeCell ref="EC1:ED1"/>
-    <mergeCell ref="EE1:EF1"/>
-    <mergeCell ref="EG1:EH1"/>
-    <mergeCell ref="EI1:EJ1"/>
-    <mergeCell ref="EK1:EL1"/>
-    <mergeCell ref="EM1:EN1"/>
-    <mergeCell ref="EO1:EP1"/>
-    <mergeCell ref="EQ1:ER1"/>
-    <mergeCell ref="ES1:ET1"/>
-    <mergeCell ref="EU1:EV1"/>
-    <mergeCell ref="EW1:EX1"/>
-    <mergeCell ref="EY1:EZ1"/>
-    <mergeCell ref="FA1:FB1"/>
-    <mergeCell ref="FC1:FD1"/>
-    <mergeCell ref="FE1:FF1"/>
-    <mergeCell ref="FG1:FH1"/>
-    <mergeCell ref="FI1:FJ1"/>
-    <mergeCell ref="FK1:FL1"/>
-    <mergeCell ref="FM1:FR1"/>
-    <mergeCell ref="FS1:FW1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>